<commit_message>
draft of new plot
</commit_message>
<xml_diff>
--- a/data/21 06 10 AgNPs fish excretion models simulations.xlsx
+++ b/data/21 06 10 AgNPs fish excretion models simulations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/AgNP-ELA_fish-excretion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="13_ncr:1_{333C23FD-339B-4120-9960-1A10164C3EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37E86ECE-378D-41B2-8979-D87E9F1593B8}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="13_ncr:1_{333C23FD-339B-4120-9960-1A10164C3EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40DE091F-B165-4C00-AEA0-CD7F56B05DF8}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1360" yWindow="2720" windowWidth="14400" windowHeight="7280" xr2:uid="{097E9588-E6E8-4050-963F-81EF450CE2DB}"/>
+    <workbookView minimized="1" xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="7270" xr2:uid="{097E9588-E6E8-4050-963F-81EF450CE2DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Fish excretion" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -541,16 +541,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -822,10 +821,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1127,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98364C61-89D6-4CA9-B9CD-6190EAD1FA66}">
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1635,11 +1630,11 @@
       <c r="B23" s="13">
         <v>2012</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="15">
         <f t="shared" ref="C23:D25" si="6">10^C17</f>
         <v>27.598392989007433</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="16">
         <f t="shared" si="6"/>
         <v>14.70194754518673</v>
       </c>
@@ -1668,11 +1663,11 @@
       <c r="B24" s="13">
         <v>2014</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="15">
         <f t="shared" si="6"/>
         <v>31.468251277957375</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="16">
         <f t="shared" si="6"/>
         <v>15.373574929434854</v>
       </c>
@@ -1698,14 +1693,14 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B25" s="15">
+      <c r="B25" s="14">
         <v>2015</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="17">
         <f t="shared" si="6"/>
         <v>17.187350184456029</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="18">
         <f t="shared" si="6"/>
         <v>11.30425406865114</v>
       </c>
@@ -1819,11 +1814,11 @@
       <c r="B34" s="13">
         <v>2012</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="15">
         <f t="shared" ref="C34:D34" si="13">10^C28</f>
         <v>1.3120933180391832</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="16">
         <f t="shared" si="13"/>
         <v>1.2748461307355781</v>
       </c>
@@ -1832,24 +1827,24 @@
       <c r="B35" s="13">
         <v>2014</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="15">
         <f t="shared" ref="C35:D35" si="14">10^C29</f>
         <v>1.3104985968296734</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="16">
         <f t="shared" si="14"/>
         <v>1.280730553112277</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="15">
+      <c r="B36" s="14">
         <v>2015</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C36" s="17">
         <f t="shared" ref="C36:D36" si="15">10^C30</f>
         <v>1.2936206918777799</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D36" s="18">
         <f t="shared" si="15"/>
         <v>1.2589955726674278</v>
       </c>
@@ -1920,11 +1915,11 @@
         <v>2012</v>
       </c>
       <c r="C48">
-        <f t="shared" ref="C48:D50" si="17">1.461+(0.684*LOG10(I12))+(0.0246*I2)-0.2013+0.7804</f>
+        <f>1.461+(0.684*LOG10(I12))+(0.0246*I2)-0.2013+0.7804</f>
         <v>2.3795327359437133</v>
       </c>
       <c r="D48">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="C48:D50" si="17">1.461+(0.684*LOG10(J12))+(0.0246*J2)-0.2013+0.7804</f>
         <v>2.0464909659316737</v>
       </c>
       <c r="E48" t="s">
@@ -2033,11 +2028,11 @@
       <c r="B58" s="13">
         <v>2012</v>
       </c>
-      <c r="C58" s="16">
+      <c r="C58" s="15">
         <f t="shared" ref="C58:D60" si="20">10^C48</f>
         <v>239.62533660375581</v>
       </c>
-      <c r="D58" s="17">
+      <c r="D58" s="16">
         <f t="shared" si="20"/>
         <v>111.29892404803986</v>
       </c>
@@ -2046,24 +2041,24 @@
       <c r="B59" s="13">
         <v>2014</v>
       </c>
-      <c r="C59" s="16">
+      <c r="C59" s="15">
         <f t="shared" si="20"/>
         <v>279.36598317422857</v>
       </c>
-      <c r="D59" s="17">
+      <c r="D59" s="16">
         <f t="shared" si="20"/>
         <v>117.78526569314698</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B60" s="15">
+      <c r="B60" s="14">
         <v>2015</v>
       </c>
-      <c r="C60" s="18">
+      <c r="C60" s="17">
         <f t="shared" si="20"/>
         <v>135.50077214099701</v>
       </c>
-      <c r="D60" s="19">
+      <c r="D60" s="18">
         <f t="shared" si="20"/>
         <v>80.784317871257329</v>
       </c>
@@ -2083,11 +2078,11 @@
       <c r="B63" s="13">
         <v>2012</v>
       </c>
-      <c r="C63" s="16">
+      <c r="C63" s="15">
         <f>10^C53</f>
         <v>1.2629570060056998</v>
       </c>
-      <c r="D63" s="16">
+      <c r="D63" s="15">
         <f>10^D53</f>
         <v>1.2337965120410657</v>
       </c>
@@ -2096,24 +2091,24 @@
       <c r="B64" s="13">
         <v>2014</v>
       </c>
-      <c r="C64" s="16">
+      <c r="C64" s="15">
         <f t="shared" ref="C64:D64" si="21">10^C54</f>
         <v>1.2635318707073291</v>
       </c>
-      <c r="D64" s="16">
+      <c r="D64" s="15">
         <f t="shared" si="21"/>
         <v>1.2377802196082091</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B65" s="15">
+      <c r="B65" s="14">
         <v>2015</v>
       </c>
-      <c r="C65" s="16">
+      <c r="C65" s="15">
         <f t="shared" ref="C65:D65" si="22">10^C55</f>
         <v>1.2466513976358702</v>
       </c>
-      <c r="D65" s="16">
+      <c r="D65" s="15">
         <f t="shared" si="22"/>
         <v>1.2214591464284597</v>
       </c>
@@ -2406,192 +2401,174 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCB1118-7300-4CD2-82A1-E1B53136AEB8}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="14">
+      <c r="A2">
         <v>2012</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2">
         <v>222</v>
       </c>
       <c r="C2">
         <v>0.65</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2">
         <v>239.62533660375581</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2">
         <v>1.2629570060056998</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2">
         <v>27.598392989007433</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2">
         <v>1.3120933180391832</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="14">
+      <c r="A3">
         <v>2014</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3">
         <v>222</v>
       </c>
       <c r="C3">
         <v>0.96</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3">
         <v>279.36598317422857</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3">
         <v>1.2635318707073291</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3">
         <v>31.468251277957375</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3">
         <v>1.3104985968296734</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="14">
+      <c r="A4">
         <v>2015</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4">
         <v>222</v>
       </c>
       <c r="C4">
         <v>0.26</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4">
         <v>135.50077214099701</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4">
         <v>1.2466513976358702</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4">
         <v>17.187350184456029</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4">
         <v>1.2936206918777799</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="14">
+      <c r="A5">
         <v>2012</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5">
         <v>239</v>
       </c>
       <c r="C5">
         <v>0.25</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5">
         <v>111.29892404803986</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5">
         <v>1.2337965120410657</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5">
         <v>14.70194754518673</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5">
         <v>1.2748461307355781</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="14">
+      <c r="A6">
         <v>2014</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6">
         <v>239</v>
       </c>
       <c r="C6">
         <v>0.25</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6">
         <v>117.78526569314698</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6">
         <v>1.2377802196082091</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6">
         <v>15.373574929434854</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6">
         <v>1.280730553112277</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="14">
+      <c r="A7">
         <v>2015</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7">
         <v>239</v>
       </c>
       <c r="C7">
         <v>0.17</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7">
         <v>80.784317871257329</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7">
         <v>1.2214591464284597</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7">
         <v>11.30425406865114</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7">
         <v>1.2589955726674278</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2603,7 +2580,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2615,136 +2592,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2">
         <v>19</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2">
         <v>0.65</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14" t="s">
+      <c r="B3" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3">
         <v>17</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3">
         <v>0.25</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="A4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4">
         <v>20</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4">
         <v>0.96</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14" t="s">
+      <c r="B5" t="s">
         <v>73</v>
       </c>
       <c r="C5">
         <v>17</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5">
         <v>0.25</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="A6" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" t="s">
         <v>72</v>
       </c>
       <c r="C6">
         <v>18</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6">
         <v>0.26</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="19" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14" t="s">
+      <c r="B7" t="s">
         <v>73</v>
       </c>
       <c r="C7">
         <v>16</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7">
         <v>0.17</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>